<commit_message>
changing datasheet and README
</commit_message>
<xml_diff>
--- a/DataSpread/data.xlsx
+++ b/DataSpread/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,6 +428,7 @@
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -438,7 +439,37 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Data collected @ Sat Jul 15 10:43:16 2023.txt</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 10:43:16 2023.txt</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 11:06:46 2023.txt</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Aug 3 8:10:15 2023.txt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Data collected @ Sat Jul 89 10:55:15 2023.txt</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 10:45:05 2023.txt</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 10:55:15 2023.txt</t>
         </is>
       </c>
     </row>
@@ -450,7 +481,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>10:43:21</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10:43:21</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>11:07:01</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12:55:28</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>8:25:22</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10:45:10</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>10:55:22</t>
         </is>
       </c>
     </row>
@@ -462,7 +523,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>10:43:51</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10:43:51</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>11:11:39</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>22:55:28</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>22:55:28</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10:50:49</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>10:57:15</t>
         </is>
       </c>
     </row>
@@ -474,7 +565,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>0:0:30</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0:0:30</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0:4:38</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>10:0:0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>14:30:6</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0:5:39</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0:1:53</t>
         </is>
       </c>
     </row>
@@ -485,7 +606,25 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="n">
+        <v>19</v>
+      </c>
+      <c r="D5" t="n">
+        <v>70</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" t="n">
         <v>12</v>
+      </c>
+      <c r="G5" t="n">
+        <v>103</v>
+      </c>
+      <c r="H5" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -495,7 +634,25 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>39</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -505,7 +662,25 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" t="n">
+        <v>55</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" t="n">
         <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>64</v>
+      </c>
+      <c r="H7" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -517,6 +692,24 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -525,7 +718,25 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>0.008330000000000001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.008330000000000001</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.07722</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
         <v>14.50167</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.09417</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.03139</v>
       </c>
     </row>
     <row r="10">
@@ -535,7 +746,25 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>2280.91</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2280.91</v>
+      </c>
+      <c r="D10" t="n">
+        <v>906.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F10" t="n">
         <v>0.83</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1093.77</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1338.01</v>
       </c>
     </row>
     <row r="11">
@@ -545,7 +774,25 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1320.53</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1320.53</v>
+      </c>
+      <c r="D11" t="n">
+        <v>194.25</v>
+      </c>
+      <c r="E11" t="n">
         <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>414.14</v>
+      </c>
+      <c r="H11" t="n">
+        <v>637.15</v>
       </c>
     </row>
     <row r="12">
@@ -555,7 +802,25 @@
         </is>
       </c>
       <c r="B12" t="n">
+        <v>960.38</v>
+      </c>
+      <c r="C12" t="n">
+        <v>960.38</v>
+      </c>
+      <c r="D12" t="n">
+        <v>712.25</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F12" t="n">
         <v>0.83</v>
+      </c>
+      <c r="G12" t="n">
+        <v>679.62</v>
+      </c>
+      <c r="H12" t="n">
+        <v>700.86</v>
       </c>
     </row>
     <row r="13">
@@ -566,7 +831,37 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>8:25:22</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -578,7 +873,37 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>10:55:28</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -588,8 +913,38 @@
           <t>Morning Peak Total Vehicles</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>3</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -598,8 +953,38 @@
           <t>Morning Peak Total Hours</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>2.50167</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -608,8 +993,38 @@
           <t>Morning Peak Vehicles per Hour</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
         <v>1.2</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -620,7 +1035,37 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>17:55:28</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>17:55:28</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -632,7 +1077,37 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>21:12:28</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>21:12:28</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -642,8 +1117,36 @@
           <t>Night Peak Total Vehicles</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -652,8 +1155,36 @@
           <t>Night Peak Total Hours</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>3.28333</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3.28333</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -662,8 +1193,36 @@
           <t>Night Peak Vehicles per Hour</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>1.83</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional Peak Hour functionality and input
</commit_message>
<xml_diff>
--- a/DataSpread/data.xlsx
+++ b/DataSpread/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,6 +424,14 @@
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -434,12 +442,32 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Data collected @ Sat Jul 15 10:43:16 2023.txt</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 11:06:46 2023.txt</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Aug 3 8:10:15 2023.txt</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Data collected @ Sat Jul 89 10:55:15 2023.txt</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Data collected @ Sat Aug 3 8:10:15 2023.txt</t>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 10:45:05 2023.txt</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Data collected @ Sat Jul 15 10:55:15 2023.txt</t>
         </is>
       </c>
     </row>
@@ -451,12 +479,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>10:43:21</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>11:07:01</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>9:55:28</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>8:44:22</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>9:55:28</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10:45:10</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10:55:22</t>
         </is>
       </c>
     </row>
@@ -468,12 +516,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>10:43:51</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11:11:39</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>22:55:28</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>22:55:28</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10:50:49</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10:57:15</t>
         </is>
       </c>
     </row>
@@ -485,12 +553,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>0:0:30</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0:4:38</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>13:0:0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>14:11:6</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>13:0:0</t>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0:5:39</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0:1:53</t>
         </is>
       </c>
     </row>
@@ -501,10 +589,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="n">
+        <v>70</v>
+      </c>
+      <c r="D5" t="n">
         <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" t="n">
+        <v>103</v>
+      </c>
+      <c r="G5" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +614,22 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
+      <c r="F6" t="n">
+        <v>39</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -527,10 +639,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
+        <v>55</v>
+      </c>
+      <c r="D7" t="n">
         <v>13</v>
+      </c>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="n">
+        <v>64</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -545,6 +669,18 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -553,10 +689,22 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>0.008330000000000001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.07722</v>
+      </c>
+      <c r="D9" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" t="n">
         <v>14.185</v>
       </c>
-      <c r="C9" t="n">
-        <v>13</v>
+      <c r="F9" t="n">
+        <v>0.09417</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.03139</v>
       </c>
     </row>
     <row r="10">
@@ -566,10 +714,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.2</v>
+        <v>2280.91</v>
       </c>
       <c r="C10" t="n">
+        <v>906.5</v>
+      </c>
+      <c r="D10" t="n">
         <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1093.77</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1338.01</v>
       </c>
     </row>
     <row r="11">
@@ -579,10 +739,22 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1320.53</v>
+      </c>
+      <c r="C11" t="n">
+        <v>194.25</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
+      <c r="F11" t="n">
+        <v>414.14</v>
+      </c>
+      <c r="G11" t="n">
+        <v>637.15</v>
       </c>
     </row>
     <row r="12">
@@ -592,10 +764,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.13</v>
+        <v>960.38</v>
       </c>
       <c r="C12" t="n">
+        <v>712.25</v>
+      </c>
+      <c r="D12" t="n">
         <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>679.62</v>
+      </c>
+      <c r="G12" t="n">
+        <v>700.86</v>
       </c>
     </row>
     <row r="13">
@@ -614,6 +798,26 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>8:44:22</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -631,6 +835,26 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10:25:28</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -648,6 +872,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>7</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -665,6 +907,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1.685</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -682,6 +942,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -699,6 +977,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -716,6 +1012,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>7</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -733,6 +1047,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -750,6 +1082,24 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -759,12 +1109,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>17:55:28</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>17:55:28</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -776,12 +1146,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>18:55:28</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>18:55:28</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>21:12:28</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>21:12:28</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -791,11 +1181,31 @@
           <t>Night Peak Total Vehicles</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>5</v>
-      </c>
-      <c r="C24" t="n">
-        <v>5</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -804,11 +1214,31 @@
           <t>Night Peak Total Hours</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>3.28333</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.28333</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -817,11 +1247,31 @@
           <t>Night Peak Vehicles per Hour</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>5</v>
-      </c>
-      <c r="C26" t="n">
-        <v>5</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -830,11 +1280,31 @@
           <t>Night Peak Vehicles from Left</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
         <v>0</v>
       </c>
-      <c r="C27" t="n">
+      <c r="E27" t="n">
         <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -853,6 +1323,22 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D28" t="n">
+        <v>6</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -860,11 +1346,31 @@
           <t>Night Peak Vph from Left</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
         <v>0</v>
       </c>
-      <c r="C29" t="n">
+      <c r="E29" t="n">
         <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -873,11 +1379,31 @@
           <t>Night Peak Vph from Right</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>5</v>
-      </c>
-      <c r="C30" t="n">
-        <v>5</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>